<commit_message>
Added Delegate Binding for the Selection Window
</commit_message>
<xml_diff>
--- a/Design/Row Formula Calculations.xlsx
+++ b/Design/Row Formula Calculations.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cryst\Documents\Prototypes\RPGWindows\Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Francesco Corso\Documents\Prototypes\RPGWindows\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:400001_{AF9C0B90-B433-46AE-8A5C-C2DE02729972}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" activeTab="3" xr2:uid="{89C3AD10-C837-4DE9-A94A-B96F00A2D81C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Rows" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="CursorLeft" sheetId="5" r:id="rId4"/>
     <sheet name="CursorRight" sheetId="7" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -76,16 +75,16 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" textRotation="90"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -400,39 +399,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0836E7EA-34C6-4265-A77B-DC01507153EE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="U6" sqref="U6:U34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.109375" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="D2" s="1" t="s">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-    </row>
-    <row r="3" spans="2:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" spans="2:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>1</v>
       </c>
@@ -479,2018 +478,2018 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="2:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="2:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4">
-        <f>MEDIAN(1, FLOOR(($C4+D$3-1)/D$3,1), $C4)</f>
+        <f t="shared" ref="D4:R13" si="0">MEDIAN(1, FLOOR(($C4+D$3-1)/D$3,1), $C4)</f>
         <v>1</v>
       </c>
       <c r="E4">
-        <f>MEDIAN(1, FLOOR(($C4+E$3-1)/E$3,1), $C4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F4">
-        <f>MEDIAN(1, FLOOR(($C4+F$3-1)/F$3,1), $C4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G4">
-        <f>MEDIAN(1, FLOOR(($C4+G$3-1)/G$3,1), $C4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H4">
-        <f>MEDIAN(1, FLOOR(($C4+H$3-1)/H$3,1), $C4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I4">
-        <f>MEDIAN(1, FLOOR(($C4+I$3-1)/I$3,1), $C4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J4">
-        <f>MEDIAN(1, FLOOR(($C4+J$3-1)/J$3,1), $C4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K4">
-        <f>MEDIAN(1, FLOOR(($C4+K$3-1)/K$3,1), $C4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L4">
-        <f>MEDIAN(1, FLOOR(($C4+L$3-1)/L$3,1), $C4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M4">
-        <f>MEDIAN(1, FLOOR(($C4+M$3-1)/M$3,1), $C4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N4">
-        <f>MEDIAN(1, FLOOR(($C4+N$3-1)/N$3,1), $C4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O4">
-        <f>MEDIAN(1, FLOOR(($C4+O$3-1)/O$3,1), $C4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P4">
-        <f>MEDIAN(1, FLOOR(($C4+P$3-1)/P$3,1), $C4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q4">
-        <f>MEDIAN(1, FLOOR(($C4+Q$3-1)/Q$3,1), $C4)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R4">
-        <f>MEDIAN(1, FLOOR(($C4+R$3-1)/R$3,1), $C4)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B5" s="2"/>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
       <c r="C5">
         <v>2</v>
       </c>
       <c r="D5">
-        <f>MEDIAN(1, FLOOR(($C5+D$3-1)/D$3,1), $C5)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="E5">
-        <f>MEDIAN(1, FLOOR(($C5+E$3-1)/E$3,1), $C5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="F5">
-        <f>MEDIAN(1, FLOOR(($C5+F$3-1)/F$3,1), $C5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G5">
-        <f>MEDIAN(1, FLOOR(($C5+G$3-1)/G$3,1), $C5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H5">
-        <f>MEDIAN(1, FLOOR(($C5+H$3-1)/H$3,1), $C5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I5">
-        <f>MEDIAN(1, FLOOR(($C5+I$3-1)/I$3,1), $C5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J5">
-        <f>MEDIAN(1, FLOOR(($C5+J$3-1)/J$3,1), $C5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K5">
-        <f>MEDIAN(1, FLOOR(($C5+K$3-1)/K$3,1), $C5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L5">
-        <f>MEDIAN(1, FLOOR(($C5+L$3-1)/L$3,1), $C5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M5">
-        <f>MEDIAN(1, FLOOR(($C5+M$3-1)/M$3,1), $C5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N5">
-        <f>MEDIAN(1, FLOOR(($C5+N$3-1)/N$3,1), $C5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O5">
-        <f>MEDIAN(1, FLOOR(($C5+O$3-1)/O$3,1), $C5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P5">
-        <f>MEDIAN(1, FLOOR(($C5+P$3-1)/P$3,1), $C5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q5">
-        <f>MEDIAN(1, FLOOR(($C5+Q$3-1)/Q$3,1), $C5)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R5">
-        <f>MEDIAN(1, FLOOR(($C5+R$3-1)/R$3,1), $C5)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B6" s="2"/>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
       <c r="C6">
         <v>3</v>
       </c>
       <c r="D6">
-        <f>MEDIAN(1, FLOOR(($C6+D$3-1)/D$3,1), $C6)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="E6">
-        <f>MEDIAN(1, FLOOR(($C6+E$3-1)/E$3,1), $C6)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F6">
-        <f>MEDIAN(1, FLOOR(($C6+F$3-1)/F$3,1), $C6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="G6">
-        <f>MEDIAN(1, FLOOR(($C6+G$3-1)/G$3,1), $C6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H6">
-        <f>MEDIAN(1, FLOOR(($C6+H$3-1)/H$3,1), $C6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I6">
-        <f>MEDIAN(1, FLOOR(($C6+I$3-1)/I$3,1), $C6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J6">
-        <f>MEDIAN(1, FLOOR(($C6+J$3-1)/J$3,1), $C6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K6">
-        <f>MEDIAN(1, FLOOR(($C6+K$3-1)/K$3,1), $C6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L6">
-        <f>MEDIAN(1, FLOOR(($C6+L$3-1)/L$3,1), $C6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M6">
-        <f>MEDIAN(1, FLOOR(($C6+M$3-1)/M$3,1), $C6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N6">
-        <f>MEDIAN(1, FLOOR(($C6+N$3-1)/N$3,1), $C6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O6">
-        <f>MEDIAN(1, FLOOR(($C6+O$3-1)/O$3,1), $C6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P6">
-        <f>MEDIAN(1, FLOOR(($C6+P$3-1)/P$3,1), $C6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q6">
-        <f>MEDIAN(1, FLOOR(($C6+Q$3-1)/Q$3,1), $C6)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R6">
-        <f>MEDIAN(1, FLOOR(($C6+R$3-1)/R$3,1), $C6)</f>
-        <v>1</v>
-      </c>
-      <c r="U6" s="4"/>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B7" s="2"/>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U6" s="2"/>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
       <c r="C7">
         <v>4</v>
       </c>
       <c r="D7">
-        <f>MEDIAN(1, FLOOR(($C7+D$3-1)/D$3,1), $C7)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E7">
-        <f>MEDIAN(1, FLOOR(($C7+E$3-1)/E$3,1), $C7)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="F7">
-        <f>MEDIAN(1, FLOOR(($C7+F$3-1)/F$3,1), $C7)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G7">
-        <f>MEDIAN(1, FLOOR(($C7+G$3-1)/G$3,1), $C7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="H7">
-        <f>MEDIAN(1, FLOOR(($C7+H$3-1)/H$3,1), $C7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I7">
-        <f>MEDIAN(1, FLOOR(($C7+I$3-1)/I$3,1), $C7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J7">
-        <f>MEDIAN(1, FLOOR(($C7+J$3-1)/J$3,1), $C7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K7">
-        <f>MEDIAN(1, FLOOR(($C7+K$3-1)/K$3,1), $C7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L7">
-        <f>MEDIAN(1, FLOOR(($C7+L$3-1)/L$3,1), $C7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M7">
-        <f>MEDIAN(1, FLOOR(($C7+M$3-1)/M$3,1), $C7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N7">
-        <f>MEDIAN(1, FLOOR(($C7+N$3-1)/N$3,1), $C7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O7">
-        <f>MEDIAN(1, FLOOR(($C7+O$3-1)/O$3,1), $C7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P7">
-        <f>MEDIAN(1, FLOOR(($C7+P$3-1)/P$3,1), $C7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q7">
-        <f>MEDIAN(1, FLOOR(($C7+Q$3-1)/Q$3,1), $C7)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R7">
-        <f>MEDIAN(1, FLOOR(($C7+R$3-1)/R$3,1), $C7)</f>
-        <v>1</v>
-      </c>
-      <c r="U7" s="4"/>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B8" s="2"/>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U7" s="2"/>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
       <c r="C8">
         <v>5</v>
       </c>
       <c r="D8">
-        <f>MEDIAN(1, FLOOR(($C8+D$3-1)/D$3,1), $C8)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E8">
-        <f>MEDIAN(1, FLOOR(($C8+E$3-1)/E$3,1), $C8)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F8">
-        <f>MEDIAN(1, FLOOR(($C8+F$3-1)/F$3,1), $C8)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G8">
-        <f>MEDIAN(1, FLOOR(($C8+G$3-1)/G$3,1), $C8)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H8">
-        <f>MEDIAN(1, FLOOR(($C8+H$3-1)/H$3,1), $C8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="I8">
-        <f>MEDIAN(1, FLOOR(($C8+I$3-1)/I$3,1), $C8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J8">
-        <f>MEDIAN(1, FLOOR(($C8+J$3-1)/J$3,1), $C8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K8">
-        <f>MEDIAN(1, FLOOR(($C8+K$3-1)/K$3,1), $C8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L8">
-        <f>MEDIAN(1, FLOOR(($C8+L$3-1)/L$3,1), $C8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M8">
-        <f>MEDIAN(1, FLOOR(($C8+M$3-1)/M$3,1), $C8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N8">
-        <f>MEDIAN(1, FLOOR(($C8+N$3-1)/N$3,1), $C8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O8">
-        <f>MEDIAN(1, FLOOR(($C8+O$3-1)/O$3,1), $C8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P8">
-        <f>MEDIAN(1, FLOOR(($C8+P$3-1)/P$3,1), $C8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q8">
-        <f>MEDIAN(1, FLOOR(($C8+Q$3-1)/Q$3,1), $C8)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R8">
-        <f>MEDIAN(1, FLOOR(($C8+R$3-1)/R$3,1), $C8)</f>
-        <v>1</v>
-      </c>
-      <c r="U8" s="4"/>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B9" s="2"/>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U8" s="2"/>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
       <c r="C9">
         <v>6</v>
       </c>
       <c r="D9">
-        <f>MEDIAN(1, FLOOR(($C9+D$3-1)/D$3,1), $C9)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E9">
-        <f>MEDIAN(1, FLOOR(($C9+E$3-1)/E$3,1), $C9)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="F9">
-        <f>MEDIAN(1, FLOOR(($C9+F$3-1)/F$3,1), $C9)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="G9">
-        <f>MEDIAN(1, FLOOR(($C9+G$3-1)/G$3,1), $C9)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H9">
-        <f>MEDIAN(1, FLOOR(($C9+H$3-1)/H$3,1), $C9)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I9">
-        <f>MEDIAN(1, FLOOR(($C9+I$3-1)/I$3,1), $C9)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="J9">
-        <f>MEDIAN(1, FLOOR(($C9+J$3-1)/J$3,1), $C9)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K9">
-        <f>MEDIAN(1, FLOOR(($C9+K$3-1)/K$3,1), $C9)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L9">
-        <f>MEDIAN(1, FLOOR(($C9+L$3-1)/L$3,1), $C9)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M9">
-        <f>MEDIAN(1, FLOOR(($C9+M$3-1)/M$3,1), $C9)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N9">
-        <f>MEDIAN(1, FLOOR(($C9+N$3-1)/N$3,1), $C9)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O9">
-        <f>MEDIAN(1, FLOOR(($C9+O$3-1)/O$3,1), $C9)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P9">
-        <f>MEDIAN(1, FLOOR(($C9+P$3-1)/P$3,1), $C9)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q9">
-        <f>MEDIAN(1, FLOOR(($C9+Q$3-1)/Q$3,1), $C9)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R9">
-        <f>MEDIAN(1, FLOOR(($C9+R$3-1)/R$3,1), $C9)</f>
-        <v>1</v>
-      </c>
-      <c r="U9" s="4"/>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U9" s="2"/>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
       <c r="C10">
         <v>7</v>
       </c>
       <c r="D10">
-        <f>MEDIAN(1, FLOOR(($C10+D$3-1)/D$3,1), $C10)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="E10">
-        <f>MEDIAN(1, FLOOR(($C10+E$3-1)/E$3,1), $C10)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F10">
-        <f>MEDIAN(1, FLOOR(($C10+F$3-1)/F$3,1), $C10)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G10">
-        <f>MEDIAN(1, FLOOR(($C10+G$3-1)/G$3,1), $C10)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H10">
-        <f>MEDIAN(1, FLOOR(($C10+H$3-1)/H$3,1), $C10)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I10">
-        <f>MEDIAN(1, FLOOR(($C10+I$3-1)/I$3,1), $C10)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J10">
-        <f>MEDIAN(1, FLOOR(($C10+J$3-1)/J$3,1), $C10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="K10">
-        <f>MEDIAN(1, FLOOR(($C10+K$3-1)/K$3,1), $C10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L10">
-        <f>MEDIAN(1, FLOOR(($C10+L$3-1)/L$3,1), $C10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M10">
-        <f>MEDIAN(1, FLOOR(($C10+M$3-1)/M$3,1), $C10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N10">
-        <f>MEDIAN(1, FLOOR(($C10+N$3-1)/N$3,1), $C10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O10">
-        <f>MEDIAN(1, FLOOR(($C10+O$3-1)/O$3,1), $C10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P10">
-        <f>MEDIAN(1, FLOOR(($C10+P$3-1)/P$3,1), $C10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q10">
-        <f>MEDIAN(1, FLOOR(($C10+Q$3-1)/Q$3,1), $C10)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R10">
-        <f>MEDIAN(1, FLOOR(($C10+R$3-1)/R$3,1), $C10)</f>
-        <v>1</v>
-      </c>
-      <c r="U10" s="4"/>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B11" s="2"/>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U10" s="2"/>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
       <c r="C11">
         <v>8</v>
       </c>
       <c r="D11">
-        <f>MEDIAN(1, FLOOR(($C11+D$3-1)/D$3,1), $C11)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="E11">
-        <f>MEDIAN(1, FLOOR(($C11+E$3-1)/E$3,1), $C11)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="F11">
-        <f>MEDIAN(1, FLOOR(($C11+F$3-1)/F$3,1), $C11)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G11">
-        <f>MEDIAN(1, FLOOR(($C11+G$3-1)/G$3,1), $C11)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H11">
-        <f>MEDIAN(1, FLOOR(($C11+H$3-1)/H$3,1), $C11)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I11">
-        <f>MEDIAN(1, FLOOR(($C11+I$3-1)/I$3,1), $C11)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J11">
-        <f>MEDIAN(1, FLOOR(($C11+J$3-1)/J$3,1), $C11)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K11">
-        <f>MEDIAN(1, FLOOR(($C11+K$3-1)/K$3,1), $C11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L11">
-        <f>MEDIAN(1, FLOOR(($C11+L$3-1)/L$3,1), $C11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M11">
-        <f>MEDIAN(1, FLOOR(($C11+M$3-1)/M$3,1), $C11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N11">
-        <f>MEDIAN(1, FLOOR(($C11+N$3-1)/N$3,1), $C11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O11">
-        <f>MEDIAN(1, FLOOR(($C11+O$3-1)/O$3,1), $C11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P11">
-        <f>MEDIAN(1, FLOOR(($C11+P$3-1)/P$3,1), $C11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q11">
-        <f>MEDIAN(1, FLOOR(($C11+Q$3-1)/Q$3,1), $C11)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R11">
-        <f>MEDIAN(1, FLOOR(($C11+R$3-1)/R$3,1), $C11)</f>
-        <v>1</v>
-      </c>
-      <c r="U11" s="4"/>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B12" s="2"/>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U11" s="2"/>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
       <c r="C12">
         <v>9</v>
       </c>
       <c r="D12">
-        <f>MEDIAN(1, FLOOR(($C12+D$3-1)/D$3,1), $C12)</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="E12">
-        <f>MEDIAN(1, FLOOR(($C12+E$3-1)/E$3,1), $C12)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F12">
-        <f>MEDIAN(1, FLOOR(($C12+F$3-1)/F$3,1), $C12)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="G12">
-        <f>MEDIAN(1, FLOOR(($C12+G$3-1)/G$3,1), $C12)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H12">
-        <f>MEDIAN(1, FLOOR(($C12+H$3-1)/H$3,1), $C12)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I12">
-        <f>MEDIAN(1, FLOOR(($C12+I$3-1)/I$3,1), $C12)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J12">
-        <f>MEDIAN(1, FLOOR(($C12+J$3-1)/J$3,1), $C12)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K12">
-        <f>MEDIAN(1, FLOOR(($C12+K$3-1)/K$3,1), $C12)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="L12">
-        <f>MEDIAN(1, FLOOR(($C12+L$3-1)/L$3,1), $C12)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="M12">
-        <f>MEDIAN(1, FLOOR(($C12+M$3-1)/M$3,1), $C12)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N12">
-        <f>MEDIAN(1, FLOOR(($C12+N$3-1)/N$3,1), $C12)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O12">
-        <f>MEDIAN(1, FLOOR(($C12+O$3-1)/O$3,1), $C12)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P12">
-        <f>MEDIAN(1, FLOOR(($C12+P$3-1)/P$3,1), $C12)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q12">
-        <f>MEDIAN(1, FLOOR(($C12+Q$3-1)/Q$3,1), $C12)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R12">
-        <f>MEDIAN(1, FLOOR(($C12+R$3-1)/R$3,1), $C12)</f>
-        <v>1</v>
-      </c>
-      <c r="U12" s="4"/>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B13" s="2"/>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U12" s="2"/>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
       <c r="C13">
         <v>10</v>
       </c>
       <c r="D13">
-        <f>MEDIAN(1, FLOOR(($C13+D$3-1)/D$3,1), $C13)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="E13">
-        <f>MEDIAN(1, FLOOR(($C13+E$3-1)/E$3,1), $C13)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="F13">
-        <f>MEDIAN(1, FLOOR(($C13+F$3-1)/F$3,1), $C13)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="G13">
-        <f>MEDIAN(1, FLOOR(($C13+G$3-1)/G$3,1), $C13)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="H13">
-        <f>MEDIAN(1, FLOOR(($C13+H$3-1)/H$3,1), $C13)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I13">
-        <f>MEDIAN(1, FLOOR(($C13+I$3-1)/I$3,1), $C13)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J13">
-        <f>MEDIAN(1, FLOOR(($C13+J$3-1)/J$3,1), $C13)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="K13">
-        <f>MEDIAN(1, FLOOR(($C13+K$3-1)/K$3,1), $C13)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="L13">
-        <f>MEDIAN(1, FLOOR(($C13+L$3-1)/L$3,1), $C13)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="M13">
-        <f>MEDIAN(1, FLOOR(($C13+M$3-1)/M$3,1), $C13)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="N13">
-        <f>MEDIAN(1, FLOOR(($C13+N$3-1)/N$3,1), $C13)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="O13">
-        <f>MEDIAN(1, FLOOR(($C13+O$3-1)/O$3,1), $C13)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="P13">
-        <f>MEDIAN(1, FLOOR(($C13+P$3-1)/P$3,1), $C13)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q13">
-        <f>MEDIAN(1, FLOOR(($C13+Q$3-1)/Q$3,1), $C13)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="R13">
-        <f>MEDIAN(1, FLOOR(($C13+R$3-1)/R$3,1), $C13)</f>
-        <v>1</v>
-      </c>
-      <c r="U13" s="4"/>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B14" s="2"/>
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="U13" s="2"/>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
       <c r="C14">
         <v>11</v>
       </c>
       <c r="D14">
-        <f>MEDIAN(1, FLOOR(($C14+D$3-1)/D$3,1), $C14)</f>
+        <f t="shared" ref="D14:R23" si="1">MEDIAN(1, FLOOR(($C14+D$3-1)/D$3,1), $C14)</f>
         <v>11</v>
       </c>
       <c r="E14">
-        <f>MEDIAN(1, FLOOR(($C14+E$3-1)/E$3,1), $C14)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="F14">
-        <f>MEDIAN(1, FLOOR(($C14+F$3-1)/F$3,1), $C14)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="G14">
-        <f>MEDIAN(1, FLOOR(($C14+G$3-1)/G$3,1), $C14)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="H14">
-        <f>MEDIAN(1, FLOOR(($C14+H$3-1)/H$3,1), $C14)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="I14">
-        <f>MEDIAN(1, FLOOR(($C14+I$3-1)/I$3,1), $C14)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J14">
-        <f>MEDIAN(1, FLOOR(($C14+J$3-1)/J$3,1), $C14)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="K14">
-        <f>MEDIAN(1, FLOOR(($C14+K$3-1)/K$3,1), $C14)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="L14">
-        <f>MEDIAN(1, FLOOR(($C14+L$3-1)/L$3,1), $C14)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="M14">
-        <f>MEDIAN(1, FLOOR(($C14+M$3-1)/M$3,1), $C14)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="N14">
-        <f>MEDIAN(1, FLOOR(($C14+N$3-1)/N$3,1), $C14)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="O14">
-        <f>MEDIAN(1, FLOOR(($C14+O$3-1)/O$3,1), $C14)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P14">
-        <f>MEDIAN(1, FLOOR(($C14+P$3-1)/P$3,1), $C14)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q14">
-        <f>MEDIAN(1, FLOOR(($C14+Q$3-1)/Q$3,1), $C14)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R14">
-        <f>MEDIAN(1, FLOOR(($C14+R$3-1)/R$3,1), $C14)</f>
-        <v>1</v>
-      </c>
-      <c r="U14" s="4"/>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B15" s="2"/>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U14" s="2"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
       <c r="C15">
         <v>12</v>
       </c>
       <c r="D15">
-        <f>MEDIAN(1, FLOOR(($C15+D$3-1)/D$3,1), $C15)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="E15">
-        <f>MEDIAN(1, FLOOR(($C15+E$3-1)/E$3,1), $C15)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="F15">
-        <f>MEDIAN(1, FLOOR(($C15+F$3-1)/F$3,1), $C15)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="G15">
-        <f>MEDIAN(1, FLOOR(($C15+G$3-1)/G$3,1), $C15)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="H15">
-        <f>MEDIAN(1, FLOOR(($C15+H$3-1)/H$3,1), $C15)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="I15">
-        <f>MEDIAN(1, FLOOR(($C15+I$3-1)/I$3,1), $C15)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="J15">
-        <f>MEDIAN(1, FLOOR(($C15+J$3-1)/J$3,1), $C15)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="K15">
-        <f>MEDIAN(1, FLOOR(($C15+K$3-1)/K$3,1), $C15)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="L15">
-        <f>MEDIAN(1, FLOOR(($C15+L$3-1)/L$3,1), $C15)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="M15">
-        <f>MEDIAN(1, FLOOR(($C15+M$3-1)/M$3,1), $C15)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="N15">
-        <f>MEDIAN(1, FLOOR(($C15+N$3-1)/N$3,1), $C15)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="O15">
-        <f>MEDIAN(1, FLOOR(($C15+O$3-1)/O$3,1), $C15)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="P15">
-        <f>MEDIAN(1, FLOOR(($C15+P$3-1)/P$3,1), $C15)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q15">
-        <f>MEDIAN(1, FLOOR(($C15+Q$3-1)/Q$3,1), $C15)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R15">
-        <f>MEDIAN(1, FLOOR(($C15+R$3-1)/R$3,1), $C15)</f>
-        <v>1</v>
-      </c>
-      <c r="U15" s="4"/>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B16" s="2"/>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U15" s="2"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
       <c r="C16">
         <v>13</v>
       </c>
       <c r="D16">
-        <f>MEDIAN(1, FLOOR(($C16+D$3-1)/D$3,1), $C16)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="E16">
-        <f>MEDIAN(1, FLOOR(($C16+E$3-1)/E$3,1), $C16)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="F16">
-        <f>MEDIAN(1, FLOOR(($C16+F$3-1)/F$3,1), $C16)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="G16">
-        <f>MEDIAN(1, FLOOR(($C16+G$3-1)/G$3,1), $C16)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H16">
-        <f>MEDIAN(1, FLOOR(($C16+H$3-1)/H$3,1), $C16)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="I16">
-        <f>MEDIAN(1, FLOOR(($C16+I$3-1)/I$3,1), $C16)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J16">
-        <f>MEDIAN(1, FLOOR(($C16+J$3-1)/J$3,1), $C16)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="K16">
-        <f>MEDIAN(1, FLOOR(($C16+K$3-1)/K$3,1), $C16)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="L16">
-        <f>MEDIAN(1, FLOOR(($C16+L$3-1)/L$3,1), $C16)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="M16">
-        <f>MEDIAN(1, FLOOR(($C16+M$3-1)/M$3,1), $C16)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="N16">
-        <f>MEDIAN(1, FLOOR(($C16+N$3-1)/N$3,1), $C16)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="O16">
-        <f>MEDIAN(1, FLOOR(($C16+O$3-1)/O$3,1), $C16)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="P16">
-        <f>MEDIAN(1, FLOOR(($C16+P$3-1)/P$3,1), $C16)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q16">
-        <f>MEDIAN(1, FLOOR(($C16+Q$3-1)/Q$3,1), $C16)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R16">
-        <f>MEDIAN(1, FLOOR(($C16+R$3-1)/R$3,1), $C16)</f>
-        <v>1</v>
-      </c>
-      <c r="U16" s="4"/>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B17" s="2"/>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U16" s="2"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
       <c r="C17">
         <v>14</v>
       </c>
       <c r="D17">
-        <f>MEDIAN(1, FLOOR(($C17+D$3-1)/D$3,1), $C17)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="E17">
-        <f>MEDIAN(1, FLOOR(($C17+E$3-1)/E$3,1), $C17)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="F17">
-        <f>MEDIAN(1, FLOOR(($C17+F$3-1)/F$3,1), $C17)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="G17">
-        <f>MEDIAN(1, FLOOR(($C17+G$3-1)/G$3,1), $C17)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H17">
-        <f>MEDIAN(1, FLOOR(($C17+H$3-1)/H$3,1), $C17)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="I17">
-        <f>MEDIAN(1, FLOOR(($C17+I$3-1)/I$3,1), $C17)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J17">
-        <f>MEDIAN(1, FLOOR(($C17+J$3-1)/J$3,1), $C17)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="K17">
-        <f>MEDIAN(1, FLOOR(($C17+K$3-1)/K$3,1), $C17)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="L17">
-        <f>MEDIAN(1, FLOOR(($C17+L$3-1)/L$3,1), $C17)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="M17">
-        <f>MEDIAN(1, FLOOR(($C17+M$3-1)/M$3,1), $C17)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="N17">
-        <f>MEDIAN(1, FLOOR(($C17+N$3-1)/N$3,1), $C17)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="O17">
-        <f>MEDIAN(1, FLOOR(($C17+O$3-1)/O$3,1), $C17)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="P17">
-        <f>MEDIAN(1, FLOOR(($C17+P$3-1)/P$3,1), $C17)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Q17">
-        <f>MEDIAN(1, FLOOR(($C17+Q$3-1)/Q$3,1), $C17)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="R17">
-        <f>MEDIAN(1, FLOOR(($C17+R$3-1)/R$3,1), $C17)</f>
-        <v>1</v>
-      </c>
-      <c r="U17" s="4"/>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B18" s="2"/>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U17" s="2"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
       <c r="C18">
         <v>15</v>
       </c>
       <c r="D18">
-        <f>MEDIAN(1, FLOOR(($C18+D$3-1)/D$3,1), $C18)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="E18">
-        <f>MEDIAN(1, FLOOR(($C18+E$3-1)/E$3,1), $C18)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="F18">
-        <f>MEDIAN(1, FLOOR(($C18+F$3-1)/F$3,1), $C18)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="G18">
-        <f>MEDIAN(1, FLOOR(($C18+G$3-1)/G$3,1), $C18)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H18">
-        <f>MEDIAN(1, FLOOR(($C18+H$3-1)/H$3,1), $C18)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="I18">
-        <f>MEDIAN(1, FLOOR(($C18+I$3-1)/I$3,1), $C18)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J18">
-        <f>MEDIAN(1, FLOOR(($C18+J$3-1)/J$3,1), $C18)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K18">
-        <f>MEDIAN(1, FLOOR(($C18+K$3-1)/K$3,1), $C18)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="L18">
-        <f>MEDIAN(1, FLOOR(($C18+L$3-1)/L$3,1), $C18)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="M18">
-        <f>MEDIAN(1, FLOOR(($C18+M$3-1)/M$3,1), $C18)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="N18">
-        <f>MEDIAN(1, FLOOR(($C18+N$3-1)/N$3,1), $C18)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="O18">
-        <f>MEDIAN(1, FLOOR(($C18+O$3-1)/O$3,1), $C18)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="P18">
-        <f>MEDIAN(1, FLOOR(($C18+P$3-1)/P$3,1), $C18)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Q18">
-        <f>MEDIAN(1, FLOOR(($C18+Q$3-1)/Q$3,1), $C18)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="R18">
-        <f>MEDIAN(1, FLOOR(($C18+R$3-1)/R$3,1), $C18)</f>
-        <v>1</v>
-      </c>
-      <c r="U18" s="4"/>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B19" s="2"/>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="U18" s="2"/>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
       <c r="C19">
         <v>16</v>
       </c>
       <c r="D19">
-        <f>MEDIAN(1, FLOOR(($C19+D$3-1)/D$3,1), $C19)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="E19">
-        <f>MEDIAN(1, FLOOR(($C19+E$3-1)/E$3,1), $C19)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="F19">
-        <f>MEDIAN(1, FLOOR(($C19+F$3-1)/F$3,1), $C19)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="G19">
-        <f>MEDIAN(1, FLOOR(($C19+G$3-1)/G$3,1), $C19)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="H19">
-        <f>MEDIAN(1, FLOOR(($C19+H$3-1)/H$3,1), $C19)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I19">
-        <f>MEDIAN(1, FLOOR(($C19+I$3-1)/I$3,1), $C19)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J19">
-        <f>MEDIAN(1, FLOOR(($C19+J$3-1)/J$3,1), $C19)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K19">
-        <f>MEDIAN(1, FLOOR(($C19+K$3-1)/K$3,1), $C19)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="L19">
-        <f>MEDIAN(1, FLOOR(($C19+L$3-1)/L$3,1), $C19)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="M19">
-        <f>MEDIAN(1, FLOOR(($C19+M$3-1)/M$3,1), $C19)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="N19">
-        <f>MEDIAN(1, FLOOR(($C19+N$3-1)/N$3,1), $C19)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="O19">
-        <f>MEDIAN(1, FLOOR(($C19+O$3-1)/O$3,1), $C19)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="P19">
-        <f>MEDIAN(1, FLOOR(($C19+P$3-1)/P$3,1), $C19)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Q19">
-        <f>MEDIAN(1, FLOOR(($C19+Q$3-1)/Q$3,1), $C19)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="R19">
-        <f>MEDIAN(1, FLOOR(($C19+R$3-1)/R$3,1), $C19)</f>
-        <v>2</v>
-      </c>
-      <c r="U19" s="4"/>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="U19" s="2"/>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
       <c r="C20">
         <v>17</v>
       </c>
       <c r="D20">
-        <f>MEDIAN(1, FLOOR(($C20+D$3-1)/D$3,1), $C20)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="E20">
-        <f>MEDIAN(1, FLOOR(($C20+E$3-1)/E$3,1), $C20)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="F20">
-        <f>MEDIAN(1, FLOOR(($C20+F$3-1)/F$3,1), $C20)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="G20">
-        <f>MEDIAN(1, FLOOR(($C20+G$3-1)/G$3,1), $C20)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="H20">
-        <f>MEDIAN(1, FLOOR(($C20+H$3-1)/H$3,1), $C20)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I20">
-        <f>MEDIAN(1, FLOOR(($C20+I$3-1)/I$3,1), $C20)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J20">
-        <f>MEDIAN(1, FLOOR(($C20+J$3-1)/J$3,1), $C20)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K20">
-        <f>MEDIAN(1, FLOOR(($C20+K$3-1)/K$3,1), $C20)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="L20">
-        <f>MEDIAN(1, FLOOR(($C20+L$3-1)/L$3,1), $C20)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="M20">
-        <f>MEDIAN(1, FLOOR(($C20+M$3-1)/M$3,1), $C20)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="N20">
-        <f>MEDIAN(1, FLOOR(($C20+N$3-1)/N$3,1), $C20)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="O20">
-        <f>MEDIAN(1, FLOOR(($C20+O$3-1)/O$3,1), $C20)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="P20">
-        <f>MEDIAN(1, FLOOR(($C20+P$3-1)/P$3,1), $C20)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Q20">
-        <f>MEDIAN(1, FLOOR(($C20+Q$3-1)/Q$3,1), $C20)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="R20">
-        <f>MEDIAN(1, FLOOR(($C20+R$3-1)/R$3,1), $C20)</f>
-        <v>2</v>
-      </c>
-      <c r="U20" s="4"/>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="U20" s="2"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
       <c r="C21">
         <v>18</v>
       </c>
       <c r="D21">
-        <f>MEDIAN(1, FLOOR(($C21+D$3-1)/D$3,1), $C21)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="E21">
-        <f>MEDIAN(1, FLOOR(($C21+E$3-1)/E$3,1), $C21)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="F21">
-        <f>MEDIAN(1, FLOOR(($C21+F$3-1)/F$3,1), $C21)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="G21">
-        <f>MEDIAN(1, FLOOR(($C21+G$3-1)/G$3,1), $C21)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="H21">
-        <f>MEDIAN(1, FLOOR(($C21+H$3-1)/H$3,1), $C21)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I21">
-        <f>MEDIAN(1, FLOOR(($C21+I$3-1)/I$3,1), $C21)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="J21">
-        <f>MEDIAN(1, FLOOR(($C21+J$3-1)/J$3,1), $C21)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K21">
-        <f>MEDIAN(1, FLOOR(($C21+K$3-1)/K$3,1), $C21)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="L21">
-        <f>MEDIAN(1, FLOOR(($C21+L$3-1)/L$3,1), $C21)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="M21">
-        <f>MEDIAN(1, FLOOR(($C21+M$3-1)/M$3,1), $C21)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="N21">
-        <f>MEDIAN(1, FLOOR(($C21+N$3-1)/N$3,1), $C21)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="O21">
-        <f>MEDIAN(1, FLOOR(($C21+O$3-1)/O$3,1), $C21)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="P21">
-        <f>MEDIAN(1, FLOOR(($C21+P$3-1)/P$3,1), $C21)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Q21">
-        <f>MEDIAN(1, FLOOR(($C21+Q$3-1)/Q$3,1), $C21)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="R21">
-        <f>MEDIAN(1, FLOOR(($C21+R$3-1)/R$3,1), $C21)</f>
-        <v>2</v>
-      </c>
-      <c r="U21" s="4"/>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B22" s="2"/>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="U21" s="2"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
       <c r="C22">
         <v>19</v>
       </c>
       <c r="D22">
-        <f>MEDIAN(1, FLOOR(($C22+D$3-1)/D$3,1), $C22)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="E22">
-        <f>MEDIAN(1, FLOOR(($C22+E$3-1)/E$3,1), $C22)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="F22">
-        <f>MEDIAN(1, FLOOR(($C22+F$3-1)/F$3,1), $C22)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="G22">
-        <f>MEDIAN(1, FLOOR(($C22+G$3-1)/G$3,1), $C22)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="H22">
-        <f>MEDIAN(1, FLOOR(($C22+H$3-1)/H$3,1), $C22)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I22">
-        <f>MEDIAN(1, FLOOR(($C22+I$3-1)/I$3,1), $C22)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J22">
-        <f>MEDIAN(1, FLOOR(($C22+J$3-1)/J$3,1), $C22)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K22">
-        <f>MEDIAN(1, FLOOR(($C22+K$3-1)/K$3,1), $C22)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="L22">
-        <f>MEDIAN(1, FLOOR(($C22+L$3-1)/L$3,1), $C22)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="M22">
-        <f>MEDIAN(1, FLOOR(($C22+M$3-1)/M$3,1), $C22)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="N22">
-        <f>MEDIAN(1, FLOOR(($C22+N$3-1)/N$3,1), $C22)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="O22">
-        <f>MEDIAN(1, FLOOR(($C22+O$3-1)/O$3,1), $C22)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="P22">
-        <f>MEDIAN(1, FLOOR(($C22+P$3-1)/P$3,1), $C22)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Q22">
-        <f>MEDIAN(1, FLOOR(($C22+Q$3-1)/Q$3,1), $C22)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="R22">
-        <f>MEDIAN(1, FLOOR(($C22+R$3-1)/R$3,1), $C22)</f>
-        <v>2</v>
-      </c>
-      <c r="U22" s="4"/>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="U22" s="2"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
       <c r="C23">
         <v>20</v>
       </c>
       <c r="D23">
-        <f>MEDIAN(1, FLOOR(($C23+D$3-1)/D$3,1), $C23)</f>
+        <f t="shared" si="1"/>
         <v>20</v>
       </c>
       <c r="E23">
-        <f>MEDIAN(1, FLOOR(($C23+E$3-1)/E$3,1), $C23)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="F23">
-        <f>MEDIAN(1, FLOOR(($C23+F$3-1)/F$3,1), $C23)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="G23">
-        <f>MEDIAN(1, FLOOR(($C23+G$3-1)/G$3,1), $C23)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="H23">
-        <f>MEDIAN(1, FLOOR(($C23+H$3-1)/H$3,1), $C23)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="I23">
-        <f>MEDIAN(1, FLOOR(($C23+I$3-1)/I$3,1), $C23)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="J23">
-        <f>MEDIAN(1, FLOOR(($C23+J$3-1)/J$3,1), $C23)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="K23">
-        <f>MEDIAN(1, FLOOR(($C23+K$3-1)/K$3,1), $C23)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="L23">
-        <f>MEDIAN(1, FLOOR(($C23+L$3-1)/L$3,1), $C23)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="M23">
-        <f>MEDIAN(1, FLOOR(($C23+M$3-1)/M$3,1), $C23)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="N23">
-        <f>MEDIAN(1, FLOOR(($C23+N$3-1)/N$3,1), $C23)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="O23">
-        <f>MEDIAN(1, FLOOR(($C23+O$3-1)/O$3,1), $C23)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="P23">
-        <f>MEDIAN(1, FLOOR(($C23+P$3-1)/P$3,1), $C23)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Q23">
-        <f>MEDIAN(1, FLOOR(($C23+Q$3-1)/Q$3,1), $C23)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="R23">
-        <f>MEDIAN(1, FLOOR(($C23+R$3-1)/R$3,1), $C23)</f>
-        <v>2</v>
-      </c>
-      <c r="U23" s="4"/>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B24" s="2"/>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="U23" s="2"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
       <c r="C24">
         <v>21</v>
       </c>
       <c r="D24">
-        <f>MEDIAN(1, FLOOR(($C24+D$3-1)/D$3,1), $C24)</f>
+        <f t="shared" ref="D24:R33" si="2">MEDIAN(1, FLOOR(($C24+D$3-1)/D$3,1), $C24)</f>
         <v>21</v>
       </c>
       <c r="E24">
-        <f>MEDIAN(1, FLOOR(($C24+E$3-1)/E$3,1), $C24)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="F24">
-        <f>MEDIAN(1, FLOOR(($C24+F$3-1)/F$3,1), $C24)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="G24">
-        <f>MEDIAN(1, FLOOR(($C24+G$3-1)/G$3,1), $C24)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="H24">
-        <f>MEDIAN(1, FLOOR(($C24+H$3-1)/H$3,1), $C24)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I24">
-        <f>MEDIAN(1, FLOOR(($C24+I$3-1)/I$3,1), $C24)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J24">
-        <f>MEDIAN(1, FLOOR(($C24+J$3-1)/J$3,1), $C24)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="K24">
-        <f>MEDIAN(1, FLOOR(($C24+K$3-1)/K$3,1), $C24)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="L24">
-        <f>MEDIAN(1, FLOOR(($C24+L$3-1)/L$3,1), $C24)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="M24">
-        <f>MEDIAN(1, FLOOR(($C24+M$3-1)/M$3,1), $C24)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="N24">
-        <f>MEDIAN(1, FLOOR(($C24+N$3-1)/N$3,1), $C24)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="O24">
-        <f>MEDIAN(1, FLOOR(($C24+O$3-1)/O$3,1), $C24)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="P24">
-        <f>MEDIAN(1, FLOOR(($C24+P$3-1)/P$3,1), $C24)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="Q24">
-        <f>MEDIAN(1, FLOOR(($C24+Q$3-1)/Q$3,1), $C24)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="R24">
-        <f>MEDIAN(1, FLOOR(($C24+R$3-1)/R$3,1), $C24)</f>
-        <v>2</v>
-      </c>
-      <c r="U24" s="4"/>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B25" s="2"/>
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="U24" s="2"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
       <c r="C25">
         <v>22</v>
       </c>
       <c r="D25">
-        <f>MEDIAN(1, FLOOR(($C25+D$3-1)/D$3,1), $C25)</f>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="E25">
-        <f>MEDIAN(1, FLOOR(($C25+E$3-1)/E$3,1), $C25)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="F25">
-        <f>MEDIAN(1, FLOOR(($C25+F$3-1)/F$3,1), $C25)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="G25">
-        <f>MEDIAN(1, FLOOR(($C25+G$3-1)/G$3,1), $C25)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="H25">
-        <f>MEDIAN(1, FLOOR(($C25+H$3-1)/H$3,1), $C25)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I25">
-        <f>MEDIAN(1, FLOOR(($C25+I$3-1)/I$3,1), $C25)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J25">
-        <f>MEDIAN(1, FLOOR(($C25+J$3-1)/J$3,1), $C25)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="K25">
-        <f>MEDIAN(1, FLOOR(($C25+K$3-1)/K$3,1), $C25)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="L25">
-        <f>MEDIAN(1, FLOOR(($C25+L$3-1)/L$3,1), $C25)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="M25">
-        <f>MEDIAN(1, FLOOR(($C25+M$3-1)/M$3,1), $C25)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="N25">
-        <f>MEDIAN(1, FLOOR(($C25+N$3-1)/N$3,1), $C25)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="O25">
-        <f>MEDIAN(1, FLOOR(($C25+O$3-1)/O$3,1), $C25)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="P25">
-        <f>MEDIAN(1, FLOOR(($C25+P$3-1)/P$3,1), $C25)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="Q25">
-        <f>MEDIAN(1, FLOOR(($C25+Q$3-1)/Q$3,1), $C25)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="R25">
-        <f>MEDIAN(1, FLOOR(($C25+R$3-1)/R$3,1), $C25)</f>
-        <v>2</v>
-      </c>
-      <c r="U25" s="4"/>
-    </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B26" s="2"/>
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="U25" s="2"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
       <c r="C26">
         <v>23</v>
       </c>
       <c r="D26">
-        <f>MEDIAN(1, FLOOR(($C26+D$3-1)/D$3,1), $C26)</f>
+        <f t="shared" si="2"/>
         <v>23</v>
       </c>
       <c r="E26">
-        <f>MEDIAN(1, FLOOR(($C26+E$3-1)/E$3,1), $C26)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="F26">
-        <f>MEDIAN(1, FLOOR(($C26+F$3-1)/F$3,1), $C26)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="G26">
-        <f>MEDIAN(1, FLOOR(($C26+G$3-1)/G$3,1), $C26)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="H26">
-        <f>MEDIAN(1, FLOOR(($C26+H$3-1)/H$3,1), $C26)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I26">
-        <f>MEDIAN(1, FLOOR(($C26+I$3-1)/I$3,1), $C26)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J26">
-        <f>MEDIAN(1, FLOOR(($C26+J$3-1)/J$3,1), $C26)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="K26">
-        <f>MEDIAN(1, FLOOR(($C26+K$3-1)/K$3,1), $C26)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="L26">
-        <f>MEDIAN(1, FLOOR(($C26+L$3-1)/L$3,1), $C26)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="M26">
-        <f>MEDIAN(1, FLOOR(($C26+M$3-1)/M$3,1), $C26)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="N26">
-        <f>MEDIAN(1, FLOOR(($C26+N$3-1)/N$3,1), $C26)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="O26">
-        <f>MEDIAN(1, FLOOR(($C26+O$3-1)/O$3,1), $C26)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="P26">
-        <f>MEDIAN(1, FLOOR(($C26+P$3-1)/P$3,1), $C26)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="Q26">
-        <f>MEDIAN(1, FLOOR(($C26+Q$3-1)/Q$3,1), $C26)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="R26">
-        <f>MEDIAN(1, FLOOR(($C26+R$3-1)/R$3,1), $C26)</f>
-        <v>2</v>
-      </c>
-      <c r="U26" s="4"/>
-    </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B27" s="2"/>
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="U26" s="2"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
       <c r="C27">
         <v>24</v>
       </c>
       <c r="D27">
-        <f>MEDIAN(1, FLOOR(($C27+D$3-1)/D$3,1), $C27)</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="E27">
-        <f>MEDIAN(1, FLOOR(($C27+E$3-1)/E$3,1), $C27)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="F27">
-        <f>MEDIAN(1, FLOOR(($C27+F$3-1)/F$3,1), $C27)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="G27">
-        <f>MEDIAN(1, FLOOR(($C27+G$3-1)/G$3,1), $C27)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="H27">
-        <f>MEDIAN(1, FLOOR(($C27+H$3-1)/H$3,1), $C27)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I27">
-        <f>MEDIAN(1, FLOOR(($C27+I$3-1)/I$3,1), $C27)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="J27">
-        <f>MEDIAN(1, FLOOR(($C27+J$3-1)/J$3,1), $C27)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="K27">
-        <f>MEDIAN(1, FLOOR(($C27+K$3-1)/K$3,1), $C27)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="L27">
-        <f>MEDIAN(1, FLOOR(($C27+L$3-1)/L$3,1), $C27)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="M27">
-        <f>MEDIAN(1, FLOOR(($C27+M$3-1)/M$3,1), $C27)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="N27">
-        <f>MEDIAN(1, FLOOR(($C27+N$3-1)/N$3,1), $C27)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="O27">
-        <f>MEDIAN(1, FLOOR(($C27+O$3-1)/O$3,1), $C27)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="P27">
-        <f>MEDIAN(1, FLOOR(($C27+P$3-1)/P$3,1), $C27)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="Q27">
-        <f>MEDIAN(1, FLOOR(($C27+Q$3-1)/Q$3,1), $C27)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="R27">
-        <f>MEDIAN(1, FLOOR(($C27+R$3-1)/R$3,1), $C27)</f>
-        <v>2</v>
-      </c>
-      <c r="U27" s="4"/>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B28" s="2"/>
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="U27" s="2"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
       <c r="C28">
         <v>25</v>
       </c>
       <c r="D28">
-        <f>MEDIAN(1, FLOOR(($C28+D$3-1)/D$3,1), $C28)</f>
+        <f t="shared" si="2"/>
         <v>25</v>
       </c>
       <c r="E28">
-        <f>MEDIAN(1, FLOOR(($C28+E$3-1)/E$3,1), $C28)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="F28">
-        <f>MEDIAN(1, FLOOR(($C28+F$3-1)/F$3,1), $C28)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G28">
-        <f>MEDIAN(1, FLOOR(($C28+G$3-1)/G$3,1), $C28)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="H28">
-        <f>MEDIAN(1, FLOOR(($C28+H$3-1)/H$3,1), $C28)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I28">
-        <f>MEDIAN(1, FLOOR(($C28+I$3-1)/I$3,1), $C28)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="J28">
-        <f>MEDIAN(1, FLOOR(($C28+J$3-1)/J$3,1), $C28)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="K28">
-        <f>MEDIAN(1, FLOOR(($C28+K$3-1)/K$3,1), $C28)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="L28">
-        <f>MEDIAN(1, FLOOR(($C28+L$3-1)/L$3,1), $C28)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="M28">
-        <f>MEDIAN(1, FLOOR(($C28+M$3-1)/M$3,1), $C28)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="N28">
-        <f>MEDIAN(1, FLOOR(($C28+N$3-1)/N$3,1), $C28)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="O28">
-        <f>MEDIAN(1, FLOOR(($C28+O$3-1)/O$3,1), $C28)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="P28">
-        <f>MEDIAN(1, FLOOR(($C28+P$3-1)/P$3,1), $C28)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="Q28">
-        <f>MEDIAN(1, FLOOR(($C28+Q$3-1)/Q$3,1), $C28)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="R28">
-        <f>MEDIAN(1, FLOOR(($C28+R$3-1)/R$3,1), $C28)</f>
-        <v>2</v>
-      </c>
-      <c r="U28" s="4"/>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B29" s="2"/>
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="U28" s="2"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
       <c r="C29">
         <v>26</v>
       </c>
       <c r="D29">
-        <f>MEDIAN(1, FLOOR(($C29+D$3-1)/D$3,1), $C29)</f>
+        <f t="shared" si="2"/>
         <v>26</v>
       </c>
       <c r="E29">
-        <f>MEDIAN(1, FLOOR(($C29+E$3-1)/E$3,1), $C29)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="F29">
-        <f>MEDIAN(1, FLOOR(($C29+F$3-1)/F$3,1), $C29)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G29">
-        <f>MEDIAN(1, FLOOR(($C29+G$3-1)/G$3,1), $C29)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="H29">
-        <f>MEDIAN(1, FLOOR(($C29+H$3-1)/H$3,1), $C29)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I29">
-        <f>MEDIAN(1, FLOOR(($C29+I$3-1)/I$3,1), $C29)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="J29">
-        <f>MEDIAN(1, FLOOR(($C29+J$3-1)/J$3,1), $C29)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="K29">
-        <f>MEDIAN(1, FLOOR(($C29+K$3-1)/K$3,1), $C29)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="L29">
-        <f>MEDIAN(1, FLOOR(($C29+L$3-1)/L$3,1), $C29)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="M29">
-        <f>MEDIAN(1, FLOOR(($C29+M$3-1)/M$3,1), $C29)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="N29">
-        <f>MEDIAN(1, FLOOR(($C29+N$3-1)/N$3,1), $C29)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="O29">
-        <f>MEDIAN(1, FLOOR(($C29+O$3-1)/O$3,1), $C29)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="P29">
-        <f>MEDIAN(1, FLOOR(($C29+P$3-1)/P$3,1), $C29)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="Q29">
-        <f>MEDIAN(1, FLOOR(($C29+Q$3-1)/Q$3,1), $C29)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="R29">
-        <f>MEDIAN(1, FLOOR(($C29+R$3-1)/R$3,1), $C29)</f>
-        <v>2</v>
-      </c>
-      <c r="U29" s="4"/>
-    </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B30" s="2"/>
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="U29" s="2"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
       <c r="C30">
         <v>27</v>
       </c>
       <c r="D30">
-        <f>MEDIAN(1, FLOOR(($C30+D$3-1)/D$3,1), $C30)</f>
+        <f t="shared" si="2"/>
         <v>27</v>
       </c>
       <c r="E30">
-        <f>MEDIAN(1, FLOOR(($C30+E$3-1)/E$3,1), $C30)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="F30">
-        <f>MEDIAN(1, FLOOR(($C30+F$3-1)/F$3,1), $C30)</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="G30">
-        <f>MEDIAN(1, FLOOR(($C30+G$3-1)/G$3,1), $C30)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="H30">
-        <f>MEDIAN(1, FLOOR(($C30+H$3-1)/H$3,1), $C30)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I30">
-        <f>MEDIAN(1, FLOOR(($C30+I$3-1)/I$3,1), $C30)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="J30">
-        <f>MEDIAN(1, FLOOR(($C30+J$3-1)/J$3,1), $C30)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="K30">
-        <f>MEDIAN(1, FLOOR(($C30+K$3-1)/K$3,1), $C30)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="L30">
-        <f>MEDIAN(1, FLOOR(($C30+L$3-1)/L$3,1), $C30)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="M30">
-        <f>MEDIAN(1, FLOOR(($C30+M$3-1)/M$3,1), $C30)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="N30">
-        <f>MEDIAN(1, FLOOR(($C30+N$3-1)/N$3,1), $C30)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="O30">
-        <f>MEDIAN(1, FLOOR(($C30+O$3-1)/O$3,1), $C30)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="P30">
-        <f>MEDIAN(1, FLOOR(($C30+P$3-1)/P$3,1), $C30)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="Q30">
-        <f>MEDIAN(1, FLOOR(($C30+Q$3-1)/Q$3,1), $C30)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="R30">
-        <f>MEDIAN(1, FLOOR(($C30+R$3-1)/R$3,1), $C30)</f>
-        <v>2</v>
-      </c>
-      <c r="U30" s="4"/>
-    </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B31" s="2"/>
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="U30" s="2"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
       <c r="C31">
         <v>28</v>
       </c>
       <c r="D31">
-        <f>MEDIAN(1, FLOOR(($C31+D$3-1)/D$3,1), $C31)</f>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="E31">
-        <f>MEDIAN(1, FLOOR(($C31+E$3-1)/E$3,1), $C31)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="F31">
-        <f>MEDIAN(1, FLOOR(($C31+F$3-1)/F$3,1), $C31)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G31">
-        <f>MEDIAN(1, FLOOR(($C31+G$3-1)/G$3,1), $C31)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="H31">
-        <f>MEDIAN(1, FLOOR(($C31+H$3-1)/H$3,1), $C31)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I31">
-        <f>MEDIAN(1, FLOOR(($C31+I$3-1)/I$3,1), $C31)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="J31">
-        <f>MEDIAN(1, FLOOR(($C31+J$3-1)/J$3,1), $C31)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="K31">
-        <f>MEDIAN(1, FLOOR(($C31+K$3-1)/K$3,1), $C31)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="L31">
-        <f>MEDIAN(1, FLOOR(($C31+L$3-1)/L$3,1), $C31)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="M31">
-        <f>MEDIAN(1, FLOOR(($C31+M$3-1)/M$3,1), $C31)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="N31">
-        <f>MEDIAN(1, FLOOR(($C31+N$3-1)/N$3,1), $C31)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="O31">
-        <f>MEDIAN(1, FLOOR(($C31+O$3-1)/O$3,1), $C31)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="P31">
-        <f>MEDIAN(1, FLOOR(($C31+P$3-1)/P$3,1), $C31)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="Q31">
-        <f>MEDIAN(1, FLOOR(($C31+Q$3-1)/Q$3,1), $C31)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="R31">
-        <f>MEDIAN(1, FLOOR(($C31+R$3-1)/R$3,1), $C31)</f>
-        <v>2</v>
-      </c>
-      <c r="U31" s="4"/>
-    </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B32" s="2"/>
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="U31" s="2"/>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
       <c r="C32">
         <v>29</v>
       </c>
       <c r="D32">
-        <f>MEDIAN(1, FLOOR(($C32+D$3-1)/D$3,1), $C32)</f>
+        <f t="shared" si="2"/>
         <v>29</v>
       </c>
       <c r="E32">
-        <f>MEDIAN(1, FLOOR(($C32+E$3-1)/E$3,1), $C32)</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="F32">
-        <f>MEDIAN(1, FLOOR(($C32+F$3-1)/F$3,1), $C32)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G32">
-        <f>MEDIAN(1, FLOOR(($C32+G$3-1)/G$3,1), $C32)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="H32">
-        <f>MEDIAN(1, FLOOR(($C32+H$3-1)/H$3,1), $C32)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I32">
-        <f>MEDIAN(1, FLOOR(($C32+I$3-1)/I$3,1), $C32)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="J32">
-        <f>MEDIAN(1, FLOOR(($C32+J$3-1)/J$3,1), $C32)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="K32">
-        <f>MEDIAN(1, FLOOR(($C32+K$3-1)/K$3,1), $C32)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="L32">
-        <f>MEDIAN(1, FLOOR(($C32+L$3-1)/L$3,1), $C32)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="M32">
-        <f>MEDIAN(1, FLOOR(($C32+M$3-1)/M$3,1), $C32)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="N32">
-        <f>MEDIAN(1, FLOOR(($C32+N$3-1)/N$3,1), $C32)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="O32">
-        <f>MEDIAN(1, FLOOR(($C32+O$3-1)/O$3,1), $C32)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="P32">
-        <f>MEDIAN(1, FLOOR(($C32+P$3-1)/P$3,1), $C32)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="Q32">
-        <f>MEDIAN(1, FLOOR(($C32+Q$3-1)/Q$3,1), $C32)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="R32">
-        <f>MEDIAN(1, FLOOR(($C32+R$3-1)/R$3,1), $C32)</f>
-        <v>2</v>
-      </c>
-      <c r="U32" s="4"/>
-    </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B33" s="3"/>
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="U32" s="2"/>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
       <c r="C33">
         <v>30</v>
       </c>
       <c r="D33">
-        <f>MEDIAN(1, FLOOR(($C33+D$3-1)/D$3,1), $C33)</f>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="E33">
-        <f>MEDIAN(1, FLOOR(($C33+E$3-1)/E$3,1), $C33)</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="F33">
-        <f>MEDIAN(1, FLOOR(($C33+F$3-1)/F$3,1), $C33)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="G33">
-        <f>MEDIAN(1, FLOOR(($C33+G$3-1)/G$3,1), $C33)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="H33">
-        <f>MEDIAN(1, FLOOR(($C33+H$3-1)/H$3,1), $C33)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="I33">
-        <f>MEDIAN(1, FLOOR(($C33+I$3-1)/I$3,1), $C33)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="J33">
-        <f>MEDIAN(1, FLOOR(($C33+J$3-1)/J$3,1), $C33)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="K33">
-        <f>MEDIAN(1, FLOOR(($C33+K$3-1)/K$3,1), $C33)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="L33">
-        <f>MEDIAN(1, FLOOR(($C33+L$3-1)/L$3,1), $C33)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="M33">
-        <f>MEDIAN(1, FLOOR(($C33+M$3-1)/M$3,1), $C33)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="N33">
-        <f>MEDIAN(1, FLOOR(($C33+N$3-1)/N$3,1), $C33)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="O33">
-        <f>MEDIAN(1, FLOOR(($C33+O$3-1)/O$3,1), $C33)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="P33">
-        <f>MEDIAN(1, FLOOR(($C33+P$3-1)/P$3,1), $C33)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="Q33">
-        <f>MEDIAN(1, FLOOR(($C33+Q$3-1)/Q$3,1), $C33)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="R33">
-        <f>MEDIAN(1, FLOOR(($C33+R$3-1)/R$3,1), $C33)</f>
-        <v>2</v>
-      </c>
-      <c r="U33" s="4"/>
-    </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="U34" s="4"/>
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="U33" s="2"/>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U34" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2502,40 +2501,40 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00CA41F-5583-4E06-8749-159972A4B493}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.109375" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" customWidth="1"/>
-    <col min="20" max="20" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="D2" s="1" t="s">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-    </row>
-    <row r="3" spans="2:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" spans="2:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>1</v>
       </c>
@@ -2585,8 +2584,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:21" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="2:21" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C4">
@@ -2656,8 +2655,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:21" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="2"/>
+    <row r="5" spans="2:21" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
       <c r="C5">
         <v>1</v>
       </c>
@@ -2722,8 +2721,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B6" s="2"/>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
       <c r="C6">
         <v>2</v>
       </c>
@@ -2787,10 +2786,10 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="U6" s="4"/>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B7" s="2"/>
+      <c r="U6" s="2"/>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
       <c r="C7">
         <v>3</v>
       </c>
@@ -2854,10 +2853,10 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="U7" s="4"/>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B8" s="2"/>
+      <c r="U7" s="2"/>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
       <c r="C8">
         <v>4</v>
       </c>
@@ -2921,10 +2920,10 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="U8" s="4"/>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B9" s="2"/>
+      <c r="U8" s="2"/>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
       <c r="C9">
         <v>5</v>
       </c>
@@ -2988,10 +2987,10 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="U9" s="4"/>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
+      <c r="U9" s="2"/>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
       <c r="C10">
         <v>6</v>
       </c>
@@ -3055,10 +3054,10 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="U10" s="4"/>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B11" s="2"/>
+      <c r="U10" s="2"/>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
       <c r="C11">
         <v>7</v>
       </c>
@@ -3122,10 +3121,10 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="U11" s="4"/>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B12" s="2"/>
+      <c r="U11" s="2"/>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
       <c r="C12">
         <v>8</v>
       </c>
@@ -3189,10 +3188,10 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="U12" s="4"/>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B13" s="2"/>
+      <c r="U12" s="2"/>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
       <c r="C13">
         <v>9</v>
       </c>
@@ -3256,10 +3255,10 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="U13" s="4"/>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B14" s="2"/>
+      <c r="U13" s="2"/>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
       <c r="C14">
         <v>10</v>
       </c>
@@ -3323,10 +3322,10 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="U14" s="4"/>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B15" s="2"/>
+      <c r="U14" s="2"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
       <c r="C15">
         <v>11</v>
       </c>
@@ -3390,10 +3389,10 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="U15" s="4"/>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B16" s="2"/>
+      <c r="U15" s="2"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
       <c r="C16">
         <v>12</v>
       </c>
@@ -3457,10 +3456,10 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="U16" s="4"/>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B17" s="2"/>
+      <c r="U16" s="2"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
       <c r="C17">
         <v>13</v>
       </c>
@@ -3524,10 +3523,10 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="U17" s="4"/>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B18" s="2"/>
+      <c r="U17" s="2"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
       <c r="C18">
         <v>14</v>
       </c>
@@ -3591,10 +3590,10 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="U18" s="4"/>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B19" s="2"/>
+      <c r="U18" s="2"/>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
       <c r="C19">
         <v>15</v>
       </c>
@@ -3658,10 +3657,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U19" s="4"/>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
+      <c r="U19" s="2"/>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
       <c r="C20">
         <v>16</v>
       </c>
@@ -3725,10 +3724,10 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="U20" s="4"/>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
+      <c r="U20" s="2"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
       <c r="C21">
         <v>17</v>
       </c>
@@ -3792,10 +3791,10 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="U21" s="4"/>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B22" s="2"/>
+      <c r="U21" s="2"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
       <c r="C22">
         <v>18</v>
       </c>
@@ -3859,10 +3858,10 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="U22" s="4"/>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
+      <c r="U22" s="2"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
       <c r="C23">
         <v>19</v>
       </c>
@@ -3926,10 +3925,10 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="U23" s="4"/>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B24" s="2"/>
+      <c r="U23" s="2"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
       <c r="C24">
         <v>20</v>
       </c>
@@ -3993,10 +3992,10 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="U24" s="4"/>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B25" s="2"/>
+      <c r="U24" s="2"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
       <c r="C25">
         <v>21</v>
       </c>
@@ -4060,10 +4059,10 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="U25" s="4"/>
-    </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B26" s="2"/>
+      <c r="U25" s="2"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
       <c r="C26">
         <v>22</v>
       </c>
@@ -4127,10 +4126,10 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="U26" s="4"/>
-    </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B27" s="2"/>
+      <c r="U26" s="2"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
       <c r="C27">
         <v>23</v>
       </c>
@@ -4194,10 +4193,10 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="U27" s="4"/>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B28" s="2"/>
+      <c r="U27" s="2"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
       <c r="C28">
         <v>24</v>
       </c>
@@ -4261,10 +4260,10 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="U28" s="4"/>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B29" s="2"/>
+      <c r="U28" s="2"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
       <c r="C29">
         <v>25</v>
       </c>
@@ -4328,10 +4327,10 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U29" s="4"/>
-    </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B30" s="2"/>
+      <c r="U29" s="2"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
       <c r="C30">
         <v>26</v>
       </c>
@@ -4395,10 +4394,10 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="U30" s="4"/>
-    </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B31" s="2"/>
+      <c r="U30" s="2"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
       <c r="C31">
         <v>27</v>
       </c>
@@ -4462,10 +4461,10 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="U31" s="4"/>
-    </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B32" s="2"/>
+      <c r="U31" s="2"/>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
       <c r="C32">
         <v>28</v>
       </c>
@@ -4529,10 +4528,10 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="U32" s="4"/>
-    </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B33" s="2"/>
+      <c r="U32" s="2"/>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
       <c r="C33">
         <v>29</v>
       </c>
@@ -4596,10 +4595,10 @@
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="U33" s="4"/>
-    </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="U34" s="4"/>
+      <c r="U33" s="2"/>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U34" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -4611,40 +4610,40 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{667BBD9D-7B02-469D-8BF5-D04B2E4144EC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U34"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="R33" sqref="R33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.109375" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" customWidth="1"/>
-    <col min="20" max="20" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="D2" s="1" t="s">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-    </row>
-    <row r="3" spans="2:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" spans="2:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>1</v>
       </c>
@@ -4694,15 +4693,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:21" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="2:21" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:R32" si="0">IF($C4&lt;$T$4-D$3, $C4+D$3,$C4+D$3-$T$4)</f>
+        <f t="shared" ref="D4:R20" si="0">IF($C4&lt;$T$4-D$3, $C4+D$3,$C4+D$3-$T$4)</f>
         <v>1</v>
       </c>
       <c r="E4">
@@ -4765,8 +4764,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:21" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="2"/>
+    <row r="5" spans="2:21" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
       <c r="C5">
         <v>1</v>
       </c>
@@ -4831,8 +4830,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B6" s="2"/>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
       <c r="C6">
         <v>2</v>
       </c>
@@ -4896,10 +4895,10 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="U6" s="4"/>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B7" s="2"/>
+      <c r="U6" s="2"/>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
       <c r="C7">
         <v>3</v>
       </c>
@@ -4963,10 +4962,10 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="U7" s="4"/>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B8" s="2"/>
+      <c r="U7" s="2"/>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
       <c r="C8">
         <v>4</v>
       </c>
@@ -5030,10 +5029,10 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="U8" s="4"/>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B9" s="2"/>
+      <c r="U8" s="2"/>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
       <c r="C9">
         <v>5</v>
       </c>
@@ -5097,10 +5096,10 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="U9" s="4"/>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
+      <c r="U9" s="2"/>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
       <c r="C10">
         <v>6</v>
       </c>
@@ -5164,10 +5163,10 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="U10" s="4"/>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B11" s="2"/>
+      <c r="U10" s="2"/>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
       <c r="C11">
         <v>7</v>
       </c>
@@ -5231,10 +5230,10 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="U11" s="4"/>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B12" s="2"/>
+      <c r="U11" s="2"/>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
       <c r="C12">
         <v>8</v>
       </c>
@@ -5298,10 +5297,10 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="U12" s="4"/>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B13" s="2"/>
+      <c r="U12" s="2"/>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
       <c r="C13">
         <v>9</v>
       </c>
@@ -5365,10 +5364,10 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="U13" s="4"/>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B14" s="2"/>
+      <c r="U13" s="2"/>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
       <c r="C14">
         <v>10</v>
       </c>
@@ -5432,10 +5431,10 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="U14" s="4"/>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B15" s="2"/>
+      <c r="U14" s="2"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
       <c r="C15">
         <v>11</v>
       </c>
@@ -5499,10 +5498,10 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="U15" s="4"/>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B16" s="2"/>
+      <c r="U15" s="2"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
       <c r="C16">
         <v>12</v>
       </c>
@@ -5566,10 +5565,10 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="U16" s="4"/>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B17" s="2"/>
+      <c r="U16" s="2"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
       <c r="C17">
         <v>13</v>
       </c>
@@ -5633,10 +5632,10 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="U17" s="4"/>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B18" s="2"/>
+      <c r="U17" s="2"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
       <c r="C18">
         <v>14</v>
       </c>
@@ -5700,10 +5699,10 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="U18" s="4"/>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B19" s="2"/>
+      <c r="U18" s="2"/>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
       <c r="C19">
         <v>15</v>
       </c>
@@ -5767,10 +5766,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U19" s="4"/>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
+      <c r="U19" s="2"/>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
       <c r="C20">
         <v>16</v>
       </c>
@@ -5834,10 +5833,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="U20" s="4"/>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
+      <c r="U20" s="2"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
       <c r="C21">
         <v>17</v>
       </c>
@@ -5901,10 +5900,10 @@
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="U21" s="4"/>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B22" s="2"/>
+      <c r="U21" s="2"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
       <c r="C22">
         <v>18</v>
       </c>
@@ -5968,10 +5967,10 @@
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="U22" s="4"/>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
+      <c r="U22" s="2"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
       <c r="C23">
         <v>19</v>
       </c>
@@ -6035,10 +6034,10 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="U23" s="4"/>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B24" s="2"/>
+      <c r="U23" s="2"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
       <c r="C24">
         <v>20</v>
       </c>
@@ -6102,10 +6101,10 @@
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="U24" s="4"/>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B25" s="2"/>
+      <c r="U24" s="2"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
       <c r="C25">
         <v>21</v>
       </c>
@@ -6169,10 +6168,10 @@
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="U25" s="4"/>
-    </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B26" s="2"/>
+      <c r="U25" s="2"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
       <c r="C26">
         <v>22</v>
       </c>
@@ -6236,10 +6235,10 @@
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="U26" s="4"/>
-    </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B27" s="2"/>
+      <c r="U26" s="2"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
       <c r="C27">
         <v>23</v>
       </c>
@@ -6303,10 +6302,10 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="U27" s="4"/>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B28" s="2"/>
+      <c r="U27" s="2"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
       <c r="C28">
         <v>24</v>
       </c>
@@ -6370,10 +6369,10 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="U28" s="4"/>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B29" s="2"/>
+      <c r="U28" s="2"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
       <c r="C29">
         <v>25</v>
       </c>
@@ -6437,10 +6436,10 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="U29" s="4"/>
-    </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B30" s="2"/>
+      <c r="U29" s="2"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
       <c r="C30">
         <v>26</v>
       </c>
@@ -6504,10 +6503,10 @@
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="U30" s="4"/>
-    </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B31" s="2"/>
+      <c r="U30" s="2"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
       <c r="C31">
         <v>27</v>
       </c>
@@ -6571,10 +6570,10 @@
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="U31" s="4"/>
-    </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B32" s="2"/>
+      <c r="U31" s="2"/>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
       <c r="C32">
         <v>28</v>
       </c>
@@ -6638,10 +6637,10 @@
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="U32" s="4"/>
-    </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B33" s="2"/>
+      <c r="U32" s="2"/>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
       <c r="C33">
         <v>29</v>
       </c>
@@ -6705,10 +6704,10 @@
         <f>IF($C33&lt;$T$4-R$3, $C33+R$3,$C33+R$3-$T$4)</f>
         <v>14</v>
       </c>
-      <c r="U33" s="4"/>
-    </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="U34" s="4"/>
+      <c r="U33" s="2"/>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U34" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -6720,40 +6719,40 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43872BD5-A351-4052-B7C1-6797AF6D9030}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T15" sqref="T15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.109375" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" customWidth="1"/>
-    <col min="20" max="20" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="D2" s="1" t="s">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-    </row>
-    <row r="3" spans="2:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" spans="2:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>1</v>
       </c>
@@ -6803,8 +6802,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:21" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="2:21" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C4">
@@ -6874,8 +6873,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:21" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="2"/>
+    <row r="5" spans="2:21" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
       <c r="C5">
         <v>1</v>
       </c>
@@ -6940,8 +6939,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B6" s="2"/>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
       <c r="C6">
         <v>2</v>
       </c>
@@ -7005,10 +7004,10 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="U6" s="4"/>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B7" s="2"/>
+      <c r="U6" s="2"/>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
       <c r="C7">
         <v>3</v>
       </c>
@@ -7072,10 +7071,10 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="U7" s="4"/>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B8" s="2"/>
+      <c r="U7" s="2"/>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
       <c r="C8">
         <v>4</v>
       </c>
@@ -7139,10 +7138,10 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="U8" s="4"/>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B9" s="2"/>
+      <c r="U8" s="2"/>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
       <c r="C9">
         <v>5</v>
       </c>
@@ -7206,10 +7205,10 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="U9" s="4"/>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
+      <c r="U9" s="2"/>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
       <c r="C10">
         <v>6</v>
       </c>
@@ -7273,10 +7272,10 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="U10" s="4"/>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B11" s="2"/>
+      <c r="U10" s="2"/>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
       <c r="C11">
         <v>7</v>
       </c>
@@ -7340,10 +7339,10 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="U11" s="4"/>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B12" s="2"/>
+      <c r="U11" s="2"/>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
       <c r="C12">
         <v>8</v>
       </c>
@@ -7407,10 +7406,10 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="U12" s="4"/>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B13" s="2"/>
+      <c r="U12" s="2"/>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
       <c r="C13">
         <v>9</v>
       </c>
@@ -7474,10 +7473,10 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="U13" s="4"/>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B14" s="2"/>
+      <c r="U13" s="2"/>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
       <c r="C14">
         <v>10</v>
       </c>
@@ -7541,10 +7540,10 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="U14" s="4"/>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B15" s="2"/>
+      <c r="U14" s="2"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
       <c r="C15">
         <v>11</v>
       </c>
@@ -7608,10 +7607,10 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="U15" s="4"/>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B16" s="2"/>
+      <c r="U15" s="2"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
       <c r="C16">
         <v>12</v>
       </c>
@@ -7675,10 +7674,10 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="U16" s="4"/>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B17" s="2"/>
+      <c r="U16" s="2"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
       <c r="C17">
         <v>13</v>
       </c>
@@ -7742,10 +7741,10 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="U17" s="4"/>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B18" s="2"/>
+      <c r="U17" s="2"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
       <c r="C18">
         <v>14</v>
       </c>
@@ -7809,10 +7808,10 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="U18" s="4"/>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B19" s="2"/>
+      <c r="U18" s="2"/>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
       <c r="C19">
         <v>15</v>
       </c>
@@ -7876,10 +7875,10 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="U19" s="4"/>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
+      <c r="U19" s="2"/>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
       <c r="C20">
         <v>16</v>
       </c>
@@ -7943,10 +7942,10 @@
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="U20" s="4"/>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
+      <c r="U20" s="2"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
       <c r="C21">
         <v>17</v>
       </c>
@@ -8010,10 +8009,10 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="U21" s="4"/>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B22" s="2"/>
+      <c r="U21" s="2"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
       <c r="C22">
         <v>18</v>
       </c>
@@ -8077,10 +8076,10 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="U22" s="4"/>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
+      <c r="U22" s="2"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
       <c r="C23">
         <v>19</v>
       </c>
@@ -8144,10 +8143,10 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="U23" s="4"/>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B24" s="2"/>
+      <c r="U23" s="2"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
       <c r="C24">
         <v>20</v>
       </c>
@@ -8211,10 +8210,10 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="U24" s="4"/>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B25" s="2"/>
+      <c r="U24" s="2"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
       <c r="C25">
         <v>21</v>
       </c>
@@ -8278,10 +8277,10 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="U25" s="4"/>
-    </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B26" s="2"/>
+      <c r="U25" s="2"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
       <c r="C26">
         <v>22</v>
       </c>
@@ -8345,10 +8344,10 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="U26" s="4"/>
-    </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B27" s="2"/>
+      <c r="U26" s="2"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
       <c r="C27">
         <v>23</v>
       </c>
@@ -8412,10 +8411,10 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="U27" s="4"/>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B28" s="2"/>
+      <c r="U27" s="2"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
       <c r="C28">
         <v>24</v>
       </c>
@@ -8479,10 +8478,10 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="U28" s="4"/>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B29" s="2"/>
+      <c r="U28" s="2"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
       <c r="C29">
         <v>25</v>
       </c>
@@ -8546,10 +8545,10 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="U29" s="4"/>
-    </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B30" s="2"/>
+      <c r="U29" s="2"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
       <c r="C30">
         <v>26</v>
       </c>
@@ -8613,10 +8612,10 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="U30" s="4"/>
-    </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B31" s="2"/>
+      <c r="U30" s="2"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
       <c r="C31">
         <v>27</v>
       </c>
@@ -8680,10 +8679,10 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="U31" s="4"/>
-    </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B32" s="2"/>
+      <c r="U31" s="2"/>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
       <c r="C32">
         <v>28</v>
       </c>
@@ -8747,10 +8746,10 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="U32" s="4"/>
-    </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B33" s="2"/>
+      <c r="U32" s="2"/>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
       <c r="C33">
         <v>29</v>
       </c>
@@ -8814,10 +8813,10 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="U33" s="4"/>
-    </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="U34" s="4"/>
+      <c r="U33" s="2"/>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U34" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -8829,40 +8828,40 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D046517-F5B3-48BF-8FDF-08C90912EDCE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:U34"/>
   <sheetViews>
     <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D4" sqref="D4:R33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.109375" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" customWidth="1"/>
-    <col min="20" max="20" width="13.44140625" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" customWidth="1"/>
+    <col min="20" max="20" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="D2" s="1" t="s">
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-    </row>
-    <row r="3" spans="2:21" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" spans="2:21" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3">
         <v>1</v>
       </c>
@@ -8912,8 +8911,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:21" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="2:21" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C4">
@@ -8983,8 +8982,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="2:21" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="2"/>
+    <row r="5" spans="2:21" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="4"/>
       <c r="C5">
         <v>1</v>
       </c>
@@ -9049,8 +9048,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B6" s="2"/>
+    <row r="6" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B6" s="4"/>
       <c r="C6">
         <v>2</v>
       </c>
@@ -9114,10 +9113,10 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="U6" s="4"/>
-    </row>
-    <row r="7" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B7" s="2"/>
+      <c r="U6" s="2"/>
+    </row>
+    <row r="7" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
       <c r="C7">
         <v>3</v>
       </c>
@@ -9181,10 +9180,10 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="U7" s="4"/>
-    </row>
-    <row r="8" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B8" s="2"/>
+      <c r="U7" s="2"/>
+    </row>
+    <row r="8" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
       <c r="C8">
         <v>4</v>
       </c>
@@ -9248,10 +9247,10 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="U8" s="4"/>
-    </row>
-    <row r="9" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B9" s="2"/>
+      <c r="U8" s="2"/>
+    </row>
+    <row r="9" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
       <c r="C9">
         <v>5</v>
       </c>
@@ -9315,10 +9314,10 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="U9" s="4"/>
-    </row>
-    <row r="10" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B10" s="2"/>
+      <c r="U9" s="2"/>
+    </row>
+    <row r="10" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
       <c r="C10">
         <v>6</v>
       </c>
@@ -9382,10 +9381,10 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="U10" s="4"/>
-    </row>
-    <row r="11" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B11" s="2"/>
+      <c r="U10" s="2"/>
+    </row>
+    <row r="11" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
       <c r="C11">
         <v>7</v>
       </c>
@@ -9449,10 +9448,10 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="U11" s="4"/>
-    </row>
-    <row r="12" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B12" s="2"/>
+      <c r="U11" s="2"/>
+    </row>
+    <row r="12" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
       <c r="C12">
         <v>8</v>
       </c>
@@ -9516,10 +9515,10 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="U12" s="4"/>
-    </row>
-    <row r="13" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B13" s="2"/>
+      <c r="U12" s="2"/>
+    </row>
+    <row r="13" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B13" s="4"/>
       <c r="C13">
         <v>9</v>
       </c>
@@ -9583,10 +9582,10 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="U13" s="4"/>
-    </row>
-    <row r="14" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B14" s="2"/>
+      <c r="U13" s="2"/>
+    </row>
+    <row r="14" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B14" s="4"/>
       <c r="C14">
         <v>10</v>
       </c>
@@ -9650,10 +9649,10 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="U14" s="4"/>
-    </row>
-    <row r="15" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B15" s="2"/>
+      <c r="U14" s="2"/>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B15" s="4"/>
       <c r="C15">
         <v>11</v>
       </c>
@@ -9717,10 +9716,10 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="U15" s="4"/>
-    </row>
-    <row r="16" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B16" s="2"/>
+      <c r="U15" s="2"/>
+    </row>
+    <row r="16" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B16" s="4"/>
       <c r="C16">
         <v>12</v>
       </c>
@@ -9784,10 +9783,10 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="U16" s="4"/>
-    </row>
-    <row r="17" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B17" s="2"/>
+      <c r="U16" s="2"/>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B17" s="4"/>
       <c r="C17">
         <v>13</v>
       </c>
@@ -9851,10 +9850,10 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="U17" s="4"/>
-    </row>
-    <row r="18" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B18" s="2"/>
+      <c r="U17" s="2"/>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B18" s="4"/>
       <c r="C18">
         <v>14</v>
       </c>
@@ -9918,10 +9917,10 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="U18" s="4"/>
-    </row>
-    <row r="19" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B19" s="2"/>
+      <c r="U18" s="2"/>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="4"/>
       <c r="C19">
         <v>15</v>
       </c>
@@ -9985,10 +9984,10 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="U19" s="4"/>
-    </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
+      <c r="U19" s="2"/>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20" s="4"/>
       <c r="C20">
         <v>16</v>
       </c>
@@ -10052,10 +10051,10 @@
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="U20" s="4"/>
-    </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
+      <c r="U20" s="2"/>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B21" s="4"/>
       <c r="C21">
         <v>17</v>
       </c>
@@ -10119,10 +10118,10 @@
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="U21" s="4"/>
-    </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B22" s="2"/>
+      <c r="U21" s="2"/>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B22" s="4"/>
       <c r="C22">
         <v>18</v>
       </c>
@@ -10186,10 +10185,10 @@
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="U22" s="4"/>
-    </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B23" s="2"/>
+      <c r="U22" s="2"/>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B23" s="4"/>
       <c r="C23">
         <v>19</v>
       </c>
@@ -10253,10 +10252,10 @@
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="U23" s="4"/>
-    </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B24" s="2"/>
+      <c r="U23" s="2"/>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B24" s="4"/>
       <c r="C24">
         <v>20</v>
       </c>
@@ -10320,10 +10319,10 @@
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="U24" s="4"/>
-    </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B25" s="2"/>
+      <c r="U24" s="2"/>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B25" s="4"/>
       <c r="C25">
         <v>21</v>
       </c>
@@ -10387,10 +10386,10 @@
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="U25" s="4"/>
-    </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B26" s="2"/>
+      <c r="U25" s="2"/>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B26" s="4"/>
       <c r="C26">
         <v>22</v>
       </c>
@@ -10454,10 +10453,10 @@
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="U26" s="4"/>
-    </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B27" s="2"/>
+      <c r="U26" s="2"/>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B27" s="4"/>
       <c r="C27">
         <v>23</v>
       </c>
@@ -10521,10 +10520,10 @@
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="U27" s="4"/>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B28" s="2"/>
+      <c r="U27" s="2"/>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B28" s="4"/>
       <c r="C28">
         <v>24</v>
       </c>
@@ -10588,10 +10587,10 @@
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="U28" s="4"/>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B29" s="2"/>
+      <c r="U28" s="2"/>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B29" s="4"/>
       <c r="C29">
         <v>25</v>
       </c>
@@ -10655,10 +10654,10 @@
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="U29" s="4"/>
-    </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B30" s="2"/>
+      <c r="U29" s="2"/>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B30" s="4"/>
       <c r="C30">
         <v>26</v>
       </c>
@@ -10722,10 +10721,10 @@
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="U30" s="4"/>
-    </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B31" s="2"/>
+      <c r="U30" s="2"/>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B31" s="4"/>
       <c r="C31">
         <v>27</v>
       </c>
@@ -10789,10 +10788,10 @@
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="U31" s="4"/>
-    </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B32" s="2"/>
+      <c r="U31" s="2"/>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B32" s="4"/>
       <c r="C32">
         <v>28</v>
       </c>
@@ -10856,10 +10855,10 @@
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="U32" s="4"/>
-    </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="B33" s="2"/>
+      <c r="U32" s="2"/>
+    </row>
+    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B33" s="4"/>
       <c r="C33">
         <v>29</v>
       </c>
@@ -10923,10 +10922,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="U33" s="4"/>
-    </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.3">
-      <c r="U34" s="4"/>
+      <c r="U33" s="2"/>
+    </row>
+    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="U34" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>